<commit_message>
rm main from workflows f3b5f5d3ca5d9fc1f643a3bfbfbb7da9b0864959
</commit_message>
<xml_diff>
--- a/main/ig/StructureDefinition-FrBasisOfDoseComponent.xlsx
+++ b/main/ig/StructureDefinition-FrBasisOfDoseComponent.xlsx
@@ -57,7 +57,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2024-08-13T14:32:33+00:00</t>
+    <t>2024-09-03T11:48:25+00:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -1117,7 +1117,7 @@
         <v>80</v>
       </c>
       <c r="AI4" t="s" s="2">
-        <v>81</v>
+        <v>20</v>
       </c>
       <c r="AJ4" t="s" s="2">
         <v>82</v>
@@ -1325,7 +1325,7 @@
         <v>78</v>
       </c>
       <c r="AI6" t="s" s="2">
-        <v>81</v>
+        <v>20</v>
       </c>
       <c r="AJ6" t="s" s="2">
         <v>106</v>

</xml_diff>